<commit_message>
State & Events added
</commit_message>
<xml_diff>
--- a/Net Full Stack React_Plan.xlsx
+++ b/Net Full Stack React_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anami\Wipro-DotNet-React\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43B3452-11E2-4D46-B460-C5B81787B3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1E4BD2-A3D7-4083-B076-C806B4FFB9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="1" xr2:uid="{07EE2141-D745-482C-8A92-03C7DE36CEBB}"/>
   </bookViews>
@@ -810,19 +810,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1453,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8E127E-1DD1-419E-8E7D-1158858A2A87}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1567,13 +1567,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="48" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="46">
         <v>45506</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="48" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="42" t="s">
@@ -1589,7 +1589,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="47"/>
-      <c r="B8" s="50"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="47"/>
       <c r="D8" s="34" t="s">
         <v>121</v>
@@ -1671,13 +1671,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="48" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="46">
         <v>45513</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="48" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="42" t="s">
@@ -1693,7 +1693,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="47"/>
-      <c r="B14" s="50"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="47"/>
       <c r="D14" s="34" t="s">
         <v>122</v>
@@ -1830,13 +1830,13 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="51" t="s">
         <v>126</v>
       </c>
       <c r="B22" s="46">
         <v>45524</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="51" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -1850,9 +1850,9 @@
       <c r="H22" s="33"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="49"/>
+      <c r="A23" s="51"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="42" t="s">
         <v>66</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="C27" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="42" t="s">
         <v>100</v>
       </c>
       <c r="E27" s="28">
@@ -1955,7 +1955,7 @@
       <c r="C29" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="42" t="s">
         <v>114</v>
       </c>
       <c r="E29" s="28">
@@ -2167,13 +2167,13 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="51">
+      <c r="B42" s="52">
         <v>45551</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="51" t="s">
         <v>30</v>
       </c>
       <c r="D42" s="25" t="s">
@@ -2188,9 +2188,9 @@
       <c r="I42" s="33"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="49"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="49"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="51"/>
       <c r="D43" s="30" t="s">
         <v>22</v>
       </c>
@@ -2284,13 +2284,13 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="52" t="s">
+      <c r="A49" s="48" t="s">
         <v>93</v>
       </c>
       <c r="B49" s="46">
         <v>45559</v>
       </c>
-      <c r="C49" s="52" t="s">
+      <c r="C49" s="48" t="s">
         <v>33</v>
       </c>
       <c r="D49" s="30" t="s">
@@ -2307,7 +2307,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="47"/>
-      <c r="B50" s="50"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="47"/>
       <c r="D50" s="34" t="s">
         <v>125</v>
@@ -2377,24 +2377,18 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="48" t="s">
+      <c r="A54" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B54" s="48"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
       <c r="E54" s="32">
         <v>15.666666666666666</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:B23"/>
@@ -2405,6 +2399,12 @@
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Component life Cycle & React hooks
</commit_message>
<xml_diff>
--- a/Net Full Stack React_Plan.xlsx
+++ b/Net Full Stack React_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anami\Wipro-DotNet-React\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36944F21-9773-48A8-9CCB-7246EF5B4489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD38BF5B-C689-45B2-AA04-78ECF1498680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="1" xr2:uid="{07EE2141-D745-482C-8A92-03C7DE36CEBB}"/>
   </bookViews>
@@ -807,19 +807,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1450,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8E127E-1DD1-419E-8E7D-1158858A2A87}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1564,13 +1564,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="45">
         <v>45506</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="51" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="41" t="s">
@@ -1586,7 +1586,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="46"/>
-      <c r="B8" s="48"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="46"/>
       <c r="D8" s="33" t="s">
         <v>121</v>
@@ -1668,13 +1668,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="51" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="45">
         <v>45513</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="51" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="41" t="s">
@@ -1690,7 +1690,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="46"/>
-      <c r="B14" s="48"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="46"/>
       <c r="D14" s="33" t="s">
         <v>122</v>
@@ -1827,13 +1827,13 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="48" t="s">
         <v>126</v>
       </c>
       <c r="B22" s="45">
         <v>45524</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="48" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="24" t="s">
@@ -1847,9 +1847,9 @@
       <c r="H22" s="32"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="50"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="50"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="48"/>
       <c r="D23" s="41" t="s">
         <v>66</v>
       </c>
@@ -2164,13 +2164,13 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="51">
+      <c r="B42" s="50">
         <v>45551</v>
       </c>
-      <c r="C42" s="50" t="s">
+      <c r="C42" s="48" t="s">
         <v>30</v>
       </c>
       <c r="D42" s="24" t="s">
@@ -2185,9 +2185,9 @@
       <c r="I42" s="32"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="50"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="50"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="48"/>
       <c r="D43" s="29" t="s">
         <v>22</v>
       </c>
@@ -2281,13 +2281,13 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="47" t="s">
+      <c r="A49" s="51" t="s">
         <v>93</v>
       </c>
       <c r="B49" s="45">
         <v>45559</v>
       </c>
-      <c r="C49" s="47" t="s">
+      <c r="C49" s="51" t="s">
         <v>33</v>
       </c>
       <c r="D49" s="29" t="s">
@@ -2304,7 +2304,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="46"/>
-      <c r="B50" s="48"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="46"/>
       <c r="D50" s="33" t="s">
         <v>125</v>
@@ -2374,18 +2374,24 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="49" t="s">
+      <c r="A54" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B54" s="49"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="49"/>
+      <c r="B54" s="47"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
       <c r="E54" s="31">
         <v>15.666666666666666</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:B23"/>
@@ -2396,12 +2402,6 @@
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
react bootstrap & JWT added
</commit_message>
<xml_diff>
--- a/Net Full Stack React_Plan.xlsx
+++ b/Net Full Stack React_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anami\Wipro-DotNet-React\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8FD648-AD13-47F0-9A09-E3F3F043E5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88026D3-D6D2-4359-8F33-FADD5379054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="1" xr2:uid="{07EE2141-D745-482C-8A92-03C7DE36CEBB}"/>
   </bookViews>
@@ -361,9 +361,6 @@
   </si>
   <si>
     <t>Introduction to RESTful APIs, Setting Up React Application, Making HTTP Requests.</t>
-  </si>
-  <si>
-    <t>Introduction to JWT, Generating and Issuing JWT Tokens, Token Verification and Decoding</t>
   </si>
   <si>
     <t>Securing APIs with JWT Authentication, Authorizing Access with JWT</t>
@@ -515,6 +512,20 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Introduction to JWT, Generating and Issuing JWT Tokens, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Token Verification and Decoding</t>
     </r>
   </si>
 </sst>
@@ -942,19 +953,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1342,8 +1353,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1586,7 +1597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8E127E-1DD1-419E-8E7D-1158858A2A87}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
@@ -1700,13 +1711,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="49">
         <v>45506</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="51" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="40" t="s">
@@ -1722,10 +1733,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="50"/>
-      <c r="B8" s="53"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="50"/>
       <c r="D8" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" s="33">
         <v>8.3333333333333329E-2</v>
@@ -1804,13 +1815,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="51" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="49">
         <v>45513</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="51" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="40" t="s">
@@ -1826,10 +1837,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="50"/>
-      <c r="B14" s="53"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="50"/>
       <c r="D14" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E14" s="33">
         <v>8.3333333333333329E-2</v>
@@ -1847,10 +1858,10 @@
         <v>45514</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="38">
         <v>0.33333333333333331</v>
@@ -1936,10 +1947,10 @@
         <v>45521</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E20" s="38">
         <v>0.33333333333333331</v>
@@ -1963,17 +1974,17 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="52" t="s">
-        <v>122</v>
+      <c r="A22" s="54" t="s">
+        <v>121</v>
       </c>
       <c r="B22" s="49">
         <v>45524</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="54" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E22" s="25">
         <v>8.3333333333333329E-2</v>
@@ -1983,9 +1994,9 @@
       <c r="H22" s="31"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="52"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="52"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="54"/>
       <c r="D23" s="40" t="s">
         <v>66</v>
       </c>
@@ -2019,7 +2030,7 @@
         <v>45664</v>
       </c>
       <c r="M24" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N24" s="42"/>
     </row>
@@ -2049,10 +2060,10 @@
         <v>45864</v>
       </c>
       <c r="M25" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N25" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2081,10 +2092,10 @@
         <v>45731</v>
       </c>
       <c r="M26" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N26" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2113,10 +2124,10 @@
         <v>45858</v>
       </c>
       <c r="M27" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N27" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2145,7 +2156,7 @@
         <v>45745</v>
       </c>
       <c r="M28" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N28" s="42"/>
     </row>
@@ -2160,7 +2171,7 @@
         <v>36</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="27">
         <v>0.33333333333333331</v>
@@ -2193,7 +2204,7 @@
       <c r="C31" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="40" t="s">
         <v>102</v>
       </c>
       <c r="E31" s="27">
@@ -2245,7 +2256,7 @@
         <v>36</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="27">
         <v>0.33333333333333331</v>
@@ -2262,7 +2273,7 @@
         <v>39</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E35" s="27">
         <v>0.33333333333333331</v>
@@ -2279,7 +2290,7 @@
         <v>41</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E36" s="27">
         <v>0.33333333333333331</v>
@@ -2296,7 +2307,7 @@
         <v>30</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E37" s="27">
         <v>0.33333333333333331</v>
@@ -2312,7 +2323,7 @@
       <c r="C38" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="D38" s="40" t="s">
         <v>107</v>
       </c>
       <c r="E38" s="27">
@@ -2346,8 +2357,8 @@
       <c r="C40" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="26" t="s">
-        <v>108</v>
+      <c r="D40" s="40" t="s">
+        <v>127</v>
       </c>
       <c r="E40" s="27">
         <v>0.33333333333333331</v>
@@ -2363,25 +2374,25 @@
       <c r="C41" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="26" t="s">
-        <v>109</v>
+      <c r="D41" s="40" t="s">
+        <v>108</v>
       </c>
       <c r="E41" s="27">
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="52" t="s">
+      <c r="A42" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="54">
+      <c r="B42" s="55">
         <v>45551</v>
       </c>
-      <c r="C42" s="52" t="s">
+      <c r="C42" s="54" t="s">
         <v>30</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E42" s="25">
         <v>8.3333333333333329E-2</v>
@@ -2392,9 +2403,9 @@
       <c r="I42" s="31"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="52"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="52"/>
+      <c r="A43" s="54"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="54"/>
       <c r="D43" s="28" t="s">
         <v>22</v>
       </c>
@@ -2488,13 +2499,13 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="51" t="s">
         <v>93</v>
       </c>
       <c r="B49" s="49">
         <v>45559</v>
       </c>
-      <c r="C49" s="55" t="s">
+      <c r="C49" s="51" t="s">
         <v>33</v>
       </c>
       <c r="D49" s="28" t="s">
@@ -2511,19 +2522,19 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="50"/>
-      <c r="B50" s="53"/>
+      <c r="B50" s="52"/>
       <c r="C50" s="50"/>
       <c r="D50" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E50" s="33">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F50" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G50" s="31" t="s">
         <v>115</v>
-      </c>
-      <c r="G50" s="31" t="s">
-        <v>116</v>
       </c>
       <c r="H50" s="31"/>
       <c r="I50" s="31"/>
@@ -2548,7 +2559,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B52" s="19">
         <v>45561</v>
@@ -2565,7 +2576,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B53" s="19">
         <v>45562</v>
@@ -2581,24 +2592,18 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="51" t="s">
+      <c r="A54" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="B54" s="51"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
       <c r="E54" s="30">
         <v>15.666666666666666</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:B23"/>
@@ -2609,6 +2614,12 @@
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>